<commit_message>
modified:   budget_target_2425.xlsx 	modified:   filtered_hosp_data2.xlsx 	modified:   leadership_board.py 	modified:   merged_events_transactions1.xlsx 	deleted:    ~$budget_target_2425.xlsx
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DFC323-355D-5941-BB1B-BF996AC4385D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFD835-46F7-1B49-B94E-FD853C84FCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
+    <workbookView xWindow="74800" yWindow="2600" windowWidth="29400" windowHeight="19280" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
   <sheets>
     <sheet name="24.25 Budget Targets" sheetId="2" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Premier League</t>
   </si>
   <si>
-    <t>Arsenal v West Ham</t>
-  </si>
-  <si>
     <t>Arsenal Women v Tottenham Hotspur Women</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>Arsenal v Newcastle United</t>
+  </si>
+  <si>
+    <t>Arsenal v West Ham United</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,15 +592,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1">
         <v>113800</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1">
         <v>113800</v>
@@ -619,10 +619,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1">
         <v>43860</v>
@@ -630,10 +630,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>28636</v>
@@ -641,10 +641,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
         <v>52632</v>
@@ -652,10 +652,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1">
         <v>10000</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
         <v>38182</v>
@@ -674,10 +674,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1">
         <v>48256</v>
@@ -685,10 +685,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>10000</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1">
         <v>38182</v>
@@ -707,10 +707,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
         <v>10000</v>
@@ -718,10 +718,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>52632</v>
@@ -732,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1">
         <v>469797</v>
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1">
         <v>319462</v>
@@ -751,10 +751,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
         <v>380000</v>
@@ -762,10 +762,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1">
         <v>199265</v>
@@ -773,10 +773,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1">
         <v>199265</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1">
         <v>199265</v>
@@ -798,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1">
         <v>469797</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1">
         <v>490113</v>
@@ -820,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1">
         <v>390059</v>
@@ -828,10 +828,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>394122</v>
@@ -842,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1">
         <v>588136</v>
@@ -853,7 +853,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1">
         <v>492653</v>
@@ -864,7 +864,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="1">
         <v>588136</v>
@@ -872,10 +872,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1">
         <v>490113</v>
@@ -886,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1">
         <v>492653</v>
@@ -897,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1">
         <v>390059</v>
@@ -908,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1">
         <v>807500</v>
@@ -919,7 +919,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1">
         <v>617500</v>
@@ -927,10 +927,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1">
         <v>285000</v>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
         <v>807500</v>
@@ -952,7 +952,7 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1">
         <v>617500</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
modified:   budget_target_2425.xlsx 	modified:   leadership_board.py
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFD835-46F7-1B49-B94E-FD853C84FCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C502F9-2254-954B-A6A0-7513B8A922E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="74800" yWindow="2600" windowWidth="29400" windowHeight="19280" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
+    <workbookView xWindow="28960" yWindow="660" windowWidth="38080" windowHeight="19500" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
   <sheets>
     <sheet name="24.25 Budget Targets" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'24.25 Budget Targets'!$A$1:$C$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'24.25 Budget Targets'!$A$1:$C$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
   <si>
     <t>Fixture Name</t>
   </si>
@@ -179,7 +179,19 @@
     <t>Arsenal v Newcastle United</t>
   </si>
   <si>
+    <t>Arsenal Women UWCL Quarter-Final (Date TBC)</t>
+  </si>
+  <si>
+    <t>Arsenal v Fulham</t>
+  </si>
+  <si>
+    <t>Arsenal v Brentford</t>
+  </si>
+  <si>
     <t>Arsenal v West Ham United</t>
+  </si>
+  <si>
+    <t>Arsenal UEFA Champions League Round of 16</t>
   </si>
 </sst>
 </file>
@@ -243,8 +255,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{066043E1-9B4C-CF4A-9F5C-F96834F9F44D}" name="Table1" displayName="Table1" ref="A1:C37" totalsRowShown="0">
-  <autoFilter ref="A1:C37" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{066043E1-9B4C-CF4A-9F5C-F96834F9F44D}" name="Table1" displayName="Table1" ref="A1:C43" totalsRowShown="0">
+  <autoFilter ref="A1:C43" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C43">
+    <sortCondition descending="1" ref="A1:A43"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8ABEC191-56FB-3547-AABF-6D1CFED75A85}" name="EventCompetition"/>
     <tableColumn id="2" xr3:uid="{F4E9E6A5-D5F0-614E-B547-B903035C3583}" name="Fixture Name"/>
@@ -571,16 +586,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.6640625" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,134 +612,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1">
-        <v>113800</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
-        <v>113800</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1">
-        <v>43860</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>28636</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
-        <v>52632</v>
+        <v>490113</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1">
-        <v>10000</v>
+        <v>490113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
-        <v>38182</v>
+        <v>394122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>48256</v>
+        <v>490113</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>10000</v>
+        <v>285000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
-        <v>38182</v>
+        <v>570000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1">
-        <v>10000</v>
+        <v>469797</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1">
-        <v>52632</v>
+        <v>570000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -732,10 +747,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1">
-        <v>469797</v>
+        <v>807500</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,46 +766,46 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1">
-        <v>380000</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1">
-        <v>199265</v>
+        <v>469797</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1">
-        <v>199265</v>
+        <v>390059</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
-        <v>199265</v>
+        <v>588136</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -798,21 +813,21 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1">
-        <v>469797</v>
+        <v>492653</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
-        <v>490113</v>
+        <v>588136</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -820,21 +835,21 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1">
-        <v>390059</v>
+        <v>492653</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
-        <v>394122</v>
+        <v>390059</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -842,10 +857,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1">
-        <v>588136</v>
+        <v>807500</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -853,10 +868,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1">
-        <v>492653</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -864,21 +879,21 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1">
-        <v>588136</v>
+        <v>807500</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1">
-        <v>490113</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -886,109 +901,175 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1">
-        <v>492653</v>
+        <v>712500</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
-        <v>390059</v>
+        <v>113800</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1">
-        <v>807500</v>
+        <v>380000</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1">
-        <v>617500</v>
+        <v>113800</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C32" s="1">
-        <v>285000</v>
+        <v>97412</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1">
-        <v>807500</v>
+        <v>97412</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1">
-        <v>617500</v>
+        <v>199265</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C35" s="1">
-        <v>712500</v>
+        <v>199265</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1">
-        <v>97412</v>
+        <v>199265</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C37" s="1">
-        <v>97412</v>
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="1">
+        <v>28636</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="1">
+        <v>52632</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="1">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="1">
+        <v>48256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="1">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1">
+        <v>52632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   budget_target_2425.xlsx 	modified:   leaderboard_carousel.py 	modified:   rts_apps.py
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C502F9-2254-954B-A6A0-7513B8A922E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2C8E9E-A22D-904A-BFFF-8A0CE70A2F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28960" yWindow="660" windowWidth="38080" windowHeight="19500" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>Arsenal v Newcastle United</t>
   </si>
   <si>
-    <t>Arsenal Women UWCL Quarter-Final (Date TBC)</t>
-  </si>
-  <si>
     <t>Arsenal v Fulham</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>Arsenal UEFA Champions League Round of 16</t>
+  </si>
+  <si>
+    <t>Arsenal Women v Real Madrid Women</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -626,7 +626,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1">
         <v>30000</v>
@@ -659,10 +659,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1">
-        <v>490113</v>
+        <v>712500</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -736,7 +736,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1">
         <v>570000</v>
@@ -769,7 +769,7 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1">
         <v>617500</v>
@@ -890,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1">
         <v>617500</v>

</xml_diff>

<commit_message>
modified:   budget_target_2425.xlsx 	modified:   guest_portal_metrics.py
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00206759-C921-0B4D-8D5C-CD7868668E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8341C433-D5F4-8642-A225-8DE2350825D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="800" windowWidth="21260" windowHeight="14880" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
+    <workbookView xWindow="30840" yWindow="780" windowWidth="21260" windowHeight="14880" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
   <sheets>
     <sheet name="24.25 Budget Targets" sheetId="2" r:id="rId1"/>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modified:   budget_target_2425.xlsx 	new file:   guest_portal_credit_metrics.py
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3546EC9F-9227-7042-91BF-E2F6BC1CA7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CA3518-653D-E048-A17C-36113A3BA843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="24.25 Budget Targets" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'24.25 Budget Targets'!$A$1:$C$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'24.25 Budget Targets'!$A$1:$C$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>Fixture Name</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Arsenal Women v Olympique Lyonnais Féminin</t>
+  </si>
+  <si>
+    <t>Arsenal v Semi Final UCL (TBC)</t>
   </si>
 </sst>
 </file>
@@ -255,11 +258,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,10 +344,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{066043E1-9B4C-CF4A-9F5C-F96834F9F44D}" name="Table1" displayName="Table1" ref="A1:C47" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C47" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C47">
-    <sortCondition descending="1" ref="A1:A47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{066043E1-9B4C-CF4A-9F5C-F96834F9F44D}" name="Table1" displayName="Table1" ref="A1:C48" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C48" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C48">
+    <sortCondition descending="1" ref="A1:A48"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8ABEC191-56FB-3547-AABF-6D1CFED75A85}" name="EventCompetition" dataDxfId="2"/>
@@ -671,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,8 +803,8 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>53</v>
+      <c r="B11" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C11" s="2">
         <v>760000</v>
@@ -811,21 +815,21 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2">
-        <v>285000</v>
+        <v>760000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2">
-        <v>617500</v>
+        <v>285000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -833,10 +837,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2">
-        <v>570000</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -844,10 +848,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
-        <v>469797</v>
+        <v>570000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -855,10 +859,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>570000</v>
+        <v>469797</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -866,10 +870,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2">
-        <v>807500</v>
+        <v>570000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -877,10 +881,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2">
-        <v>319462</v>
+        <v>807500</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -888,10 +892,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
-        <v>617500</v>
+        <v>319462</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -899,10 +903,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2">
-        <v>469797</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -910,10 +914,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2">
-        <v>390059</v>
+        <v>469797</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -921,10 +925,10 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2">
-        <v>588136</v>
+        <v>390059</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -932,10 +936,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2">
-        <v>492653</v>
+        <v>588136</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -943,10 +947,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2">
-        <v>588136</v>
+        <v>492653</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -954,10 +958,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2">
-        <v>492653</v>
+        <v>588136</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -965,10 +969,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2">
-        <v>390059</v>
+        <v>492653</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -976,10 +980,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>807500</v>
+        <v>390059</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -987,10 +991,10 @@
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2">
-        <v>617500</v>
+        <v>807500</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -998,10 +1002,10 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C29" s="2">
-        <v>807500</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1009,10 +1013,10 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C30" s="2">
-        <v>617500</v>
+        <v>807500</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,54 +1024,54 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C31" s="2">
-        <v>712500</v>
+        <v>617500</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2">
-        <v>113800</v>
+        <v>712500</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C33" s="2">
-        <v>380000</v>
+        <v>113800</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2">
-        <v>113800</v>
+        <v>380000</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C35" s="2">
-        <v>97412</v>
+        <v>113800</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1075,7 +1079,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2">
         <v>97412</v>
@@ -1083,13 +1087,13 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C37" s="2">
-        <v>199265</v>
+        <v>97412</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1097,7 +1101,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C38" s="2">
         <v>199265</v>
@@ -1108,7 +1112,7 @@
         <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C39" s="2">
         <v>199265</v>
@@ -1116,13 +1120,13 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C40" s="2">
-        <v>52632</v>
+        <v>199265</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1130,10 +1134,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C41" s="2">
-        <v>43860</v>
+        <v>52632</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1141,10 +1145,10 @@
         <v>7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C42" s="2">
-        <v>28636</v>
+        <v>43860</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1152,10 +1156,10 @@
         <v>7</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C43" s="2">
-        <v>52632</v>
+        <v>28636</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1163,10 +1167,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C44" s="2">
-        <v>38182</v>
+        <v>52632</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1174,10 +1178,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C45" s="2">
-        <v>48256</v>
+        <v>38182</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1185,10 +1189,10 @@
         <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C46" s="2">
-        <v>38182</v>
+        <v>48256</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1196,9 +1200,20 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2">
+        <v>38182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C48" s="2">
         <v>52632</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   budget_target_2425.xlsx 	modified:   sales_performance.py 	new file:   ~$budget_target_2425.xlsx
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464A1CF-834F-2D46-878D-2E96EE856DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAC2A7F-C78B-574D-BA9D-AC3E6F846371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31520" yWindow="2000" windowWidth="28800" windowHeight="16120" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
@@ -658,7 +658,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modified:   budget_target_2425.xlsx 	modified:   leadership_board.py 	new file:   ~$budget_target_2425.xlsx
</commit_message>
<xml_diff>
--- a/budget_target_2425.xlsx
+++ b/budget_target_2425.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmunthali/Documents/PYTHON/APPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAC2A7F-C78B-574D-BA9D-AC3E6F846371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1964576-2562-7A49-8729-BE3C7239AF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31520" yWindow="2000" windowWidth="28800" windowHeight="16120" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
+    <workbookView xWindow="33320" yWindow="820" windowWidth="32680" windowHeight="18120" xr2:uid="{322D1251-3F46-2848-B295-F20D3EBD7724}"/>
   </bookViews>
   <sheets>
     <sheet name="24.25 Budget Targets" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="64">
   <si>
     <t>Fixture Name</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Arsenal Women v Vålerenga Women</t>
+  </si>
+  <si>
+    <t>Robbie Williams Live 2025 (Saturday)</t>
   </si>
 </sst>
 </file>
@@ -657,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995DD8E3-8446-B443-9BCB-9D0C4C075302}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1181,7 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C37" s="4">
         <v>45815.6875</v>

</xml_diff>